<commit_message>
preparing for new_dev branch
</commit_message>
<xml_diff>
--- a/extra/work_log.xlsx
+++ b/extra/work_log.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\awwk\Pers\pers_dev\lotopy\extra\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{A19B2654-4CF1-46FB-AFC7-74F8C4D3C705}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B431B009-418A-46C3-B2B8-209199D03522}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="40">
   <si>
     <t>Task</t>
   </si>
@@ -137,6 +137,15 @@
   </si>
   <si>
     <t>Implement connectors object</t>
+  </si>
+  <si>
+    <t>New objects to define wining combinations</t>
+  </si>
+  <si>
+    <t>New object to compare 2 results and determine wining combination</t>
+  </si>
+  <si>
+    <t>ResultComparer</t>
   </si>
 </sst>
 </file>
@@ -454,10 +463,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E24"/>
+  <dimension ref="A1:E26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A18" sqref="A18"/>
+      <selection activeCell="C25" sqref="C25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -837,6 +846,28 @@
         <v>9</v>
       </c>
     </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>37</v>
+      </c>
+      <c r="B25" t="s">
+        <v>39</v>
+      </c>
+      <c r="C25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>38</v>
+      </c>
+      <c r="B26" t="s">
+        <v>39</v>
+      </c>
+      <c r="C26">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>